<commit_message>
Actualizada última boleta 14-enero
</commit_message>
<xml_diff>
--- a/Contabilidad nueva.xlsx
+++ b/Contabilidad nueva.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Compra</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Cristobal</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>Caja electrónica</t>
+  </si>
+  <si>
+    <t>Arirang</t>
   </si>
 </sst>
 </file>
@@ -385,16 +394,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -700,7 +709,7 @@
   <dimension ref="A4:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,18 +812,18 @@
         <v>1800</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" ref="I6:I13" si="0">E6-H6</f>
+        <f t="shared" ref="I6:I14" si="0">E6-H6</f>
         <v>0</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="16">
-        <f>I7+I13</f>
-        <v>23280</v>
+      <c r="N6" s="14">
+        <f>I7+I13+I14</f>
+        <v>24420</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -846,11 +855,11 @@
         <f t="shared" si="0"/>
         <v>8310</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="15" t="s">
+      <c r="L7" s="17"/>
+      <c r="M7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="15">
         <f>I11+I12</f>
         <v>1900</v>
       </c>
@@ -1036,15 +1045,34 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="4"/>
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2">
+        <v>42018</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1140</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>1140</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>

</xml_diff>